<commit_message>
Fixed Function entersummary and enterdescription
</commit_message>
<xml_diff>
--- a/testData/defectTabTestData/defectTestCaseTab_testData.xlsx
+++ b/testData/defectTabTestData/defectTestCaseTab_testData.xlsx
@@ -1,25 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29523"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MohitAman\Desktop\UAT_NEXTNEXT_BLAZE_FRAMEWORK_AUTO\testData\defectTabTestData\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F527581B-F0BB-4606-BB25-A37BC73ADF4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6F23B137-EBD1-418F-877A-7E111F72FBBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3520" yWindow="2810" windowWidth="14400" windowHeight="7270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="tc009" sheetId="2" r:id="rId1"/>
+    <sheet name="tc009" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
@@ -27,29 +34,29 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
+    <t>Url</t>
+  </si>
+  <si>
     <t>Summary</t>
   </si>
   <si>
     <t>Description</t>
   </si>
   <si>
+    <t>https://webapp-stg-testnext.azurewebsites.net/defect</t>
+  </si>
+  <si>
     <t>Testing Summary</t>
   </si>
   <si>
     <t>Testing Description</t>
-  </si>
-  <si>
-    <t>Url</t>
-  </si>
-  <si>
-    <t>https://webapp-stg-testnext.azurewebsites.net/defect</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -61,12 +68,6 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -95,7 +96,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -430,46 +431,57 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27236CE2-700C-45C9-8A56-668FEA3A117F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="46.26953125" customWidth="1"/>
-    <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="16.90625" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
+      <c r="C2" t="s">
         <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{87B6CBD2-1E91-4FF2-88E0-5AE0ED63CFFF}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{938664A6-98D0-4D67-82A6-5216F9BEBF97}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{984425FB-E0ED-4499-9F06-D56178AE2B8E}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added TC019 , TC021 , TC022
</commit_message>
<xml_diff>
--- a/testData/defectTabTestData/defectTestCaseTab_testData.xlsx
+++ b/testData/defectTabTestData/defectTestCaseTab_testData.xlsx
@@ -3,12 +3,22 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29523"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{11A26C76-ECE8-4DC9-897F-9BDA9750DACC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D5CD78CE-9942-499F-9F42-E22930C93B1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="9" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="tc009" sheetId="1" r:id="rId1"/>
+    <sheet name="tc014" sheetId="6" r:id="rId2"/>
+    <sheet name="tc015" sheetId="7" r:id="rId3"/>
+    <sheet name="tc010" sheetId="2" r:id="rId4"/>
+    <sheet name="tc006" sheetId="3" r:id="rId5"/>
+    <sheet name="tc008" sheetId="5" r:id="rId6"/>
+    <sheet name="tc007" sheetId="8" r:id="rId7"/>
+    <sheet name="tc004" sheetId="4" r:id="rId8"/>
+    <sheet name="tc016" sheetId="9" r:id="rId9"/>
+    <sheet name="tc017" sheetId="10" r:id="rId10"/>
+    <sheet name="tc021" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -30,15 +40,226 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="50">
+  <si>
+    <t>Url</t>
+  </si>
+  <si>
+    <t>Summary</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>https://webapp-stg-testnext.azurewebsites.net/defect</t>
+  </si>
+  <si>
+    <t>Testing Summary</t>
+  </si>
+  <si>
+    <t>Testing Description</t>
+  </si>
+  <si>
+    <t>url</t>
+  </si>
+  <si>
+    <t>esummary</t>
+  </si>
+  <si>
+    <t>Summaries</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>msg</t>
+  </si>
+  <si>
+    <t>New</t>
+  </si>
+  <si>
+    <t>Defect created successfully.</t>
+  </si>
+  <si>
+    <t>Defect_id</t>
+  </si>
+  <si>
+    <t>DF-311</t>
+  </si>
+  <si>
+    <t>Affected_release</t>
+  </si>
+  <si>
+    <t>Severity</t>
+  </si>
+  <si>
+    <t>FixedR</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Module</t>
+  </si>
+  <si>
+    <t>Reason</t>
+  </si>
+  <si>
+    <t>Cat</t>
+  </si>
+  <si>
+    <t>assignedTo</t>
+  </si>
+  <si>
+    <t>target</t>
+  </si>
+  <si>
+    <t>priority</t>
+  </si>
+  <si>
+    <t>SET- DRV</t>
+  </si>
+  <si>
+    <t>Minor</t>
+  </si>
+  <si>
+    <t>Bug</t>
+  </si>
+  <si>
+    <t>MD-297 SET- DRIV</t>
+  </si>
+  <si>
+    <t>Duplicate</t>
+  </si>
+  <si>
+    <t>Design - UI</t>
+  </si>
+  <si>
+    <t>Vivek Rajput</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>project</t>
+  </si>
+  <si>
+    <t>summary</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>reason</t>
+  </si>
+  <si>
+    <t>STG- SPARK Modernization</t>
+  </si>
+  <si>
+    <t>Summariliyyy</t>
+  </si>
+  <si>
+    <t>Undecided</t>
+  </si>
+  <si>
+    <t>Abhi Suresh Nitnaware</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Assign To</t>
+  </si>
+  <si>
+    <t>Requirement - Wrong</t>
+  </si>
+  <si>
+    <t>Mohit Aman</t>
+  </si>
+  <si>
+    <t>defectId</t>
+  </si>
+  <si>
+    <t>multilineDescription</t>
+  </si>
+  <si>
+    <t>Role used :
+Steps to reproduce :
+Expected result :
+Actual result :
+User name : Sohail Shaikh
+Test data (if any) :
+Test case number : Line 3: New line added
+Line 4: End of Description</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -58,13 +279,27 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -397,12 +632,828 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="41.7109375" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{938664A6-98D0-4D67-82A6-5216F9BEBF97}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87E5D401-1490-449E-9C0A-3DF35853EE92}">
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="9" max="9" width="29.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" t="s">
+        <v>46</v>
+      </c>
+      <c r="I2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{B9D4C0EB-7FDD-4EC8-8600-7F09218EAE8D}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41609440-00B7-4122-9080-D2BC0A433D51}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="60.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="115.5">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57C9431D-5367-4EBD-BB7D-638E4D59A5BF}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{95739FB7-D7F2-409C-8597-E9D2267B148E}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F176698D-2844-4849-825F-67D3B337053C}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{172E0C13-61F9-4032-BF55-C665681D7995}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{984425FB-E0ED-4499-9F06-D56178AE2B8E}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="30.85546875" customWidth="1"/>
+    <col min="2" max="2" width="30" customWidth="1"/>
+    <col min="3" max="3" width="22.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{CFA4C855-DE38-4355-86BF-026061729869}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F11C9F18-0D54-4C96-BED8-DE87C1369977}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{2526BF51-A6FB-47A9-8E2C-36ED1636F3F4}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62D6A461-64F3-42C2-B275-475DA0075823}">
+  <dimension ref="A1:CW2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P14" sqref="P14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:101">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
+      <c r="R1" s="5"/>
+      <c r="S1" s="5"/>
+      <c r="T1" s="5"/>
+      <c r="U1" s="5"/>
+      <c r="V1" s="5"/>
+      <c r="W1" s="5"/>
+      <c r="X1" s="5"/>
+      <c r="Y1" s="5"/>
+      <c r="Z1" s="5"/>
+      <c r="AA1" s="5"/>
+      <c r="AB1" s="5"/>
+      <c r="AC1" s="5"/>
+      <c r="AD1" s="5"/>
+      <c r="AE1" s="5"/>
+      <c r="AF1" s="5"/>
+      <c r="AG1" s="5"/>
+      <c r="AH1" s="5"/>
+      <c r="AI1" s="5"/>
+      <c r="AJ1" s="5"/>
+      <c r="AK1" s="5"/>
+      <c r="AL1" s="5"/>
+      <c r="AM1" s="5"/>
+      <c r="AN1" s="5"/>
+      <c r="AO1" s="5"/>
+      <c r="AP1" s="5"/>
+      <c r="AQ1" s="5"/>
+      <c r="AR1" s="5"/>
+      <c r="AS1" s="5"/>
+      <c r="AT1" s="5"/>
+      <c r="AU1" s="5"/>
+      <c r="AV1" s="5"/>
+      <c r="AW1" s="5"/>
+      <c r="AX1" s="5"/>
+      <c r="AY1" s="5"/>
+      <c r="AZ1" s="5"/>
+      <c r="BA1" s="5"/>
+      <c r="BB1" s="5"/>
+      <c r="BC1" s="5"/>
+      <c r="BD1" s="5"/>
+      <c r="BE1" s="5"/>
+      <c r="BF1" s="5"/>
+      <c r="BG1" s="5"/>
+      <c r="BH1" s="5"/>
+      <c r="BI1" s="5"/>
+      <c r="BJ1" s="5"/>
+      <c r="BK1" s="5"/>
+      <c r="BL1" s="5"/>
+      <c r="BM1" s="5"/>
+      <c r="BN1" s="5"/>
+      <c r="BO1" s="5"/>
+      <c r="BP1" s="5"/>
+      <c r="BQ1" s="5"/>
+      <c r="BR1" s="5"/>
+      <c r="BS1" s="5"/>
+      <c r="BT1" s="5"/>
+      <c r="BU1" s="5"/>
+      <c r="BV1" s="5"/>
+      <c r="BW1" s="5"/>
+      <c r="BX1" s="5"/>
+      <c r="BY1" s="5"/>
+      <c r="BZ1" s="5"/>
+      <c r="CA1" s="5"/>
+      <c r="CB1" s="5"/>
+      <c r="CC1" s="5"/>
+      <c r="CD1" s="5"/>
+      <c r="CE1" s="5"/>
+      <c r="CF1" s="5"/>
+      <c r="CG1" s="5"/>
+      <c r="CH1" s="5"/>
+      <c r="CI1" s="5"/>
+      <c r="CJ1" s="5"/>
+      <c r="CK1" s="5"/>
+      <c r="CL1" s="5"/>
+      <c r="CM1" s="5"/>
+      <c r="CN1" s="5"/>
+      <c r="CO1" s="5"/>
+      <c r="CP1" s="5"/>
+      <c r="CQ1" s="5"/>
+      <c r="CR1" s="5"/>
+      <c r="CS1" s="5"/>
+      <c r="CT1" s="5"/>
+      <c r="CU1" s="5"/>
+      <c r="CV1" s="5"/>
+      <c r="CW1" s="5"/>
+    </row>
+    <row r="2" spans="1:101">
+      <c r="A2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5"/>
+      <c r="S2" s="5"/>
+      <c r="T2" s="5"/>
+      <c r="U2" s="5"/>
+      <c r="V2" s="5"/>
+      <c r="W2" s="5"/>
+      <c r="X2" s="5"/>
+      <c r="Y2" s="5"/>
+      <c r="Z2" s="5"/>
+      <c r="AA2" s="5"/>
+      <c r="AB2" s="5"/>
+      <c r="AC2" s="5"/>
+      <c r="AD2" s="5"/>
+      <c r="AE2" s="5"/>
+      <c r="AF2" s="5"/>
+      <c r="AG2" s="5"/>
+      <c r="AH2" s="5"/>
+      <c r="AI2" s="5"/>
+      <c r="AJ2" s="5"/>
+      <c r="AK2" s="5"/>
+      <c r="AL2" s="5"/>
+      <c r="AM2" s="5"/>
+      <c r="AN2" s="5"/>
+      <c r="AO2" s="5"/>
+      <c r="AP2" s="5"/>
+      <c r="AQ2" s="5"/>
+      <c r="AR2" s="5"/>
+      <c r="AS2" s="5"/>
+      <c r="AT2" s="5"/>
+      <c r="AU2" s="5"/>
+      <c r="AV2" s="5"/>
+      <c r="AW2" s="5"/>
+      <c r="AX2" s="5"/>
+      <c r="AY2" s="5"/>
+      <c r="AZ2" s="5"/>
+      <c r="BA2" s="5"/>
+      <c r="BB2" s="5"/>
+      <c r="BC2" s="5"/>
+      <c r="BD2" s="5"/>
+      <c r="BE2" s="5"/>
+      <c r="BF2" s="5"/>
+      <c r="BG2" s="5"/>
+      <c r="BH2" s="5"/>
+      <c r="BI2" s="5"/>
+      <c r="BJ2" s="5"/>
+      <c r="BK2" s="5"/>
+      <c r="BL2" s="5"/>
+      <c r="BM2" s="5"/>
+      <c r="BN2" s="5"/>
+      <c r="BO2" s="5"/>
+      <c r="BP2" s="5"/>
+      <c r="BQ2" s="5"/>
+      <c r="BR2" s="5"/>
+      <c r="BS2" s="5"/>
+      <c r="BT2" s="5"/>
+      <c r="BU2" s="5"/>
+      <c r="BV2" s="5"/>
+      <c r="BW2" s="5"/>
+      <c r="BX2" s="5"/>
+      <c r="BY2" s="5"/>
+      <c r="BZ2" s="5"/>
+      <c r="CA2" s="5"/>
+      <c r="CB2" s="5"/>
+      <c r="CC2" s="5"/>
+      <c r="CD2" s="5"/>
+      <c r="CE2" s="5"/>
+      <c r="CF2" s="5"/>
+      <c r="CG2" s="5"/>
+      <c r="CH2" s="5"/>
+      <c r="CI2" s="5"/>
+      <c r="CJ2" s="5"/>
+      <c r="CK2" s="5"/>
+      <c r="CL2" s="5"/>
+      <c r="CM2" s="5"/>
+      <c r="CN2" s="5"/>
+      <c r="CO2" s="5"/>
+      <c r="CP2" s="5"/>
+      <c r="CQ2" s="5"/>
+      <c r="CR2" s="5"/>
+      <c r="CS2" s="5"/>
+      <c r="CT2" s="5"/>
+      <c r="CU2" s="5"/>
+      <c r="CV2" s="5"/>
+      <c r="CW2" s="5"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{86519965-BD60-4BF3-8DFF-B92F34FD1A3E}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4800AC7E-F153-4191-9E90-3380C12B1430}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{98773125-5332-4379-98B8-0FD3F271177C}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DBB4210-9285-4E78-B062-C70F95124B52}">
+  <dimension ref="A1:G10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="10"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="10"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="10"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="10"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="10"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="10"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="10"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="10"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3D4B51D-576B-4DA1-BDAE-6F85096314D0}">
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="44.42578125" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" customWidth="1"/>
+    <col min="5" max="5" width="20.140625" customWidth="1"/>
+    <col min="8" max="8" width="14" customWidth="1"/>
+    <col min="9" max="9" width="18.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" t="s">
+        <v>46</v>
+      </c>
+      <c r="I2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{79DE2057-255F-4088-8F5E-0E08F75750CC}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added XML and testdata
</commit_message>
<xml_diff>
--- a/testData/defectTabTestData/defectTestCaseTab_testData.xlsx
+++ b/testData/defectTabTestData/defectTestCaseTab_testData.xlsx
@@ -1,56 +1,161 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29530"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MohitAman\Desktop\UAT_NEXTNEXT_BLAZE_FRAMEWORK_AUTO\testData\defectTabTestData\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85F148D1-0B3D-4F08-AC44-EB59DC3EC3FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3B2D8BDE-07FE-496F-9A29-0CAFA7BB937E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="2" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="18" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="tc009" sheetId="1" r:id="rId1"/>
-    <sheet name="tc014" sheetId="6" r:id="rId2"/>
-    <sheet name="tc015" sheetId="7" r:id="rId3"/>
-    <sheet name="tc010" sheetId="2" r:id="rId4"/>
-    <sheet name="tc006" sheetId="3" r:id="rId5"/>
-    <sheet name="tc008" sheetId="5" r:id="rId6"/>
-    <sheet name="tc007" sheetId="8" r:id="rId7"/>
-    <sheet name="tc004" sheetId="4" r:id="rId8"/>
+    <sheet name="tc004" sheetId="4" r:id="rId1"/>
+    <sheet name="tc006" sheetId="3" r:id="rId2"/>
+    <sheet name="tc007" sheetId="8" r:id="rId3"/>
+    <sheet name="tc008" sheetId="5" r:id="rId4"/>
+    <sheet name="tc009" sheetId="1" r:id="rId5"/>
+    <sheet name="tc010" sheetId="2" r:id="rId6"/>
+    <sheet name="tc014" sheetId="6" r:id="rId7"/>
+    <sheet name="tc015" sheetId="7" r:id="rId8"/>
     <sheet name="tc016" sheetId="9" r:id="rId9"/>
     <sheet name="tc017" sheetId="10" r:id="rId10"/>
-    <sheet name="tc021" sheetId="11" r:id="rId11"/>
-    <sheet name="tc041" sheetId="12" r:id="rId12"/>
-    <sheet name="tc042" sheetId="13" r:id="rId13"/>
+    <sheet name="tc018" sheetId="17" r:id="rId11"/>
+    <sheet name="tc021" sheetId="11" r:id="rId12"/>
+    <sheet name="tc023" sheetId="12" r:id="rId13"/>
+    <sheet name="tc026" sheetId="15" r:id="rId14"/>
+    <sheet name="tc027" sheetId="20" r:id="rId15"/>
+    <sheet name="tc029" sheetId="13" r:id="rId16"/>
+    <sheet name="tc030" sheetId="14" r:id="rId17"/>
+    <sheet name="tc041" sheetId="16" r:id="rId18"/>
+    <sheet name="tc047" sheetId="18" r:id="rId19"/>
+    <sheet name="tc037" sheetId="24" r:id="rId20"/>
+    <sheet name="tc046" sheetId="19" r:id="rId21"/>
+    <sheet name="tc042" sheetId="23" r:id="rId22"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="85">
+  <si>
+    <t>project</t>
+  </si>
+  <si>
+    <t>summary</t>
+  </si>
+  <si>
+    <t>priority</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>reason</t>
+  </si>
+  <si>
+    <t>assignedTo</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>STG- SPARK Modernization</t>
+  </si>
+  <si>
+    <t>Summariliyyy</t>
+  </si>
+  <si>
+    <t>Undecided</t>
+  </si>
+  <si>
+    <t>Bug</t>
+  </si>
+  <si>
+    <t>Duplicate</t>
+  </si>
+  <si>
+    <t>Abhi Suresh Nitnaware</t>
+  </si>
+  <si>
+    <t>New</t>
+  </si>
   <si>
     <t>Url</t>
   </si>
   <si>
+    <t>Defect_id</t>
+  </si>
+  <si>
+    <t>https://webapp-stg-testnext.azurewebsites.net/defect</t>
+  </si>
+  <si>
+    <t>DF-311</t>
+  </si>
+  <si>
+    <t>Affected_release</t>
+  </si>
+  <si>
+    <t>Severity</t>
+  </si>
+  <si>
+    <t>FixedR</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Module</t>
+  </si>
+  <si>
+    <t>Reason</t>
+  </si>
+  <si>
+    <t>Cat</t>
+  </si>
+  <si>
+    <t>target</t>
+  </si>
+  <si>
+    <t>SET- DRV</t>
+  </si>
+  <si>
+    <t>Minor</t>
+  </si>
+  <si>
+    <t>MD-297 SET- DRIV</t>
+  </si>
+  <si>
+    <t>Design - UI</t>
+  </si>
+  <si>
+    <t>Vivek Rajput</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
     <t>Summary</t>
   </si>
   <si>
     <t>Description</t>
   </si>
   <si>
-    <t>https://webapp-stg-testnext.azurewebsites.net/defect</t>
-  </si>
-  <si>
     <t>Testing Summary</t>
   </si>
   <si>
@@ -66,100 +171,10 @@
     <t>Summaries</t>
   </si>
   <si>
-    <t>status</t>
-  </si>
-  <si>
     <t>msg</t>
   </si>
   <si>
-    <t>New</t>
-  </si>
-  <si>
     <t>Defect created successfully.</t>
-  </si>
-  <si>
-    <t>Defect_id</t>
-  </si>
-  <si>
-    <t>DF-311</t>
-  </si>
-  <si>
-    <t>Affected_release</t>
-  </si>
-  <si>
-    <t>Severity</t>
-  </si>
-  <si>
-    <t>FixedR</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>Module</t>
-  </si>
-  <si>
-    <t>Reason</t>
-  </si>
-  <si>
-    <t>Cat</t>
-  </si>
-  <si>
-    <t>assignedTo</t>
-  </si>
-  <si>
-    <t>target</t>
-  </si>
-  <si>
-    <t>priority</t>
-  </si>
-  <si>
-    <t>SET- DRV</t>
-  </si>
-  <si>
-    <t>Minor</t>
-  </si>
-  <si>
-    <t>Bug</t>
-  </si>
-  <si>
-    <t>MD-297 SET- DRIV</t>
-  </si>
-  <si>
-    <t>Duplicate</t>
-  </si>
-  <si>
-    <t>Design - UI</t>
-  </si>
-  <si>
-    <t>Vivek Rajput</t>
-  </si>
-  <si>
-    <t>Low</t>
-  </si>
-  <si>
-    <t>project</t>
-  </si>
-  <si>
-    <t>summary</t>
-  </si>
-  <si>
-    <t>type</t>
-  </si>
-  <si>
-    <t>reason</t>
-  </si>
-  <si>
-    <t>STG- SPARK Modernization</t>
-  </si>
-  <si>
-    <t>Summariliyyy</t>
-  </si>
-  <si>
-    <t>Undecided</t>
-  </si>
-  <si>
-    <t>Abhi Suresh Nitnaware</t>
   </si>
   <si>
     <t>Category</t>
@@ -190,29 +205,134 @@
 Steps to reproduce :
 Expected result :
 Actual result :
-User name : Sohail Shaikh
+User name : Mohit Aman
 Test data (if any) :
 Test case number : Line 3: New line added
 Line 4: End of Description</t>
   </si>
   <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>expectedSummary</t>
+  </si>
+  <si>
+    <t>expectedAffectedRelease</t>
+  </si>
+  <si>
+    <t>expectedSeverity</t>
+  </si>
+  <si>
+    <t>expectedFixedRelease</t>
+  </si>
+  <si>
+    <t>expectedType</t>
+  </si>
+  <si>
+    <t>expectedModule</t>
+  </si>
+  <si>
+    <t>expectedReason</t>
+  </si>
+  <si>
+    <t>expectedCategory</t>
+  </si>
+  <si>
+    <t>expectedAssignTo</t>
+  </si>
+  <si>
+    <t>expectedTargetRelease</t>
+  </si>
+  <si>
+    <t>expectedStatus</t>
+  </si>
+  <si>
+    <t>expectedPriority</t>
+  </si>
+  <si>
+    <t>expectedDescription</t>
+  </si>
+  <si>
+    <t>-- Select Affected Release --</t>
+  </si>
+  <si>
+    <t>-- Select Severity --</t>
+  </si>
+  <si>
+    <t>-- Select Fixed Release --</t>
+  </si>
+  <si>
+    <t>-- Select Type --</t>
+  </si>
+  <si>
+    <t>-- Select Module --</t>
+  </si>
+  <si>
+    <t>-- Select Reason --</t>
+  </si>
+  <si>
+    <t>-- Select Category --</t>
+  </si>
+  <si>
+    <t>-- Select Target Release --</t>
+  </si>
+  <si>
+    <t>-- Select Status --</t>
+  </si>
+  <si>
+    <t>-- Select Priority --</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Role used :
+Steps to reproduce :
+Expected result :
+Actual result :
+User name : Mohit Aman
+Test data (if any) :
+Test case number : </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Role used :
+Steps to reproduce :
+Expected result :
+Actual result :
+User name :
+Test data (if any) :
+Test case number : </t>
+  </si>
+  <si>
     <t>ID</t>
   </si>
   <si>
+    <t>ID1</t>
+  </si>
+  <si>
     <t>DF-1</t>
   </si>
   <si>
     <t xml:space="preserve">   Testing Summary</t>
   </si>
   <si>
-    <t>ID1</t>
+    <t>####</t>
+  </si>
+  <si>
+    <t>&amp;&amp;&amp;&amp;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">status </t>
+  </si>
+  <si>
+    <t>testcase Summary</t>
+  </si>
+  <si>
+    <t>Automation Description</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -230,7 +350,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -260,7 +380,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -271,6 +391,17 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF242424"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -278,7 +409,20 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -303,7 +447,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -318,7 +462,22 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -653,45 +812,134 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DBB4210-9285-4E78-B062-C70F95124B52}">
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="41.7265625" customWidth="1"/>
-    <col min="2" max="2" width="21.1796875" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
+      <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="E1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="F1" s="10" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="10"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="10"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="10"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="10"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="10"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="10"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="10"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="10"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{938664A6-98D0-4D67-82A6-5216F9BEBF97}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -701,26 +949,26 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection sqref="A1:I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="9" max="9" width="29.1796875" customWidth="1"/>
+    <col min="9" max="9" width="29.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9">
       <c r="A1" s="9" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="C1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E1" t="s">
         <v>41</v>
@@ -735,36 +983,36 @@
         <v>44</v>
       </c>
       <c r="I1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>4</v>
+        <v>34</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D2" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="E2" t="s">
         <v>45</v>
       </c>
       <c r="F2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="H2" t="s">
         <v>46</v>
       </c>
       <c r="I2" t="s">
-        <v>5</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -776,19 +1024,100 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41609440-00B7-4122-9080-D2BC0A433D51}">
-  <dimension ref="A1:B2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B310B858-FEFA-48A5-B995-DA133501E07F}">
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="60.453125" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" customWidth="1"/>
+    <col min="8" max="8" width="17.140625" customWidth="1"/>
+    <col min="9" max="9" width="27.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9">
+      <c r="A1" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" t="s">
+        <v>46</v>
+      </c>
+      <c r="I2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{AB19A363-286C-4679-8DCD-0C56253EB022}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41609440-00B7-4122-9080-D2BC0A433D51}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5:D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="60.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>47</v>
       </c>
@@ -796,236 +1125,396 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="116" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" ht="115.5">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>49</v>
       </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="D5" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8B649E1-B7F5-45AB-B6F3-CC5B4D1A5F59}">
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3259BD86-3F8F-4A42-86F4-5DD744C41E44}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C2"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56806B28-3978-47F9-8A2E-A1FAB993CEA2}">
+  <dimension ref="A1:N2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="25.42578125" defaultRowHeight="55.5" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="19.7265625" customWidth="1"/>
-    <col min="3" max="3" width="20.7265625" customWidth="1"/>
+    <col min="1" max="16384" width="25.42578125" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:14" ht="55.5" customHeight="1">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="H1" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="I1" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="J1" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="K1" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="L1" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="M1" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1" s="15" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="55.5" customHeight="1">
+      <c r="A2" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="15"/>
+      <c r="C2" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="I2" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="J2" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="K2" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="L2" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="M2" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="N2" s="15" t="s">
+        <v>74</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8D2FA3B-A385-40DB-B8F7-3AD897BAF126}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C1" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:4" ht="216.75">
+      <c r="A2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>75</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAA3B7BB-8D47-428A-AFA2-8FBE09983B20}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>51</v>
+        <v>16</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{A36F8F8B-8B89-45D3-88E6-6612C1C4AEB5}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{37AC72DE-8FBE-4EDB-8A35-CE96D7521365}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59AB94A0-26C0-4BA7-8A0A-78C8277DEBD7}">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="46.6328125" customWidth="1"/>
-    <col min="2" max="2" width="14" customWidth="1"/>
-    <col min="3" max="3" width="19.7265625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>52</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{11F94A12-9768-4137-9408-BCF9B1B0A914}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57C9431D-5367-4EBD-BB7D-638E4D59A5BF}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="A1" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{95739FB7-D7F2-409C-8597-E9D2267B148E}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F176698D-2844-4849-825F-67D3B337053C}">
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{291E5E8B-3DC4-459B-886A-59328C11C1BB}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4">
       <c r="A1" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>9</v>
-      </c>
       <c r="D1" s="8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.35">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{172E0C13-61F9-4032-BF55-C665681D7995}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{6784271E-276C-4D31-8375-14BA890EE7FF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{984425FB-E0ED-4499-9F06-D56178AE2B8E}">
-  <dimension ref="A1:C2"/>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC29B807-E3D5-449A-8A03-0861456EF643}">
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView topLeftCell="K1" workbookViewId="0">
+      <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="30.81640625" customWidth="1"/>
-    <col min="2" max="2" width="30" customWidth="1"/>
-    <col min="3" max="3" width="22.453125" customWidth="1"/>
+    <col min="1" max="1" width="50.85546875" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" customWidth="1"/>
+    <col min="3" max="3" width="27.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>5</v>
+    <row r="1" spans="1:4">
+      <c r="A1" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{CFA4C855-DE38-4355-86BF-026061729869}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{C4C735ED-C70C-4B58-8CAD-3C000986EACA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4399D2F9-CD9F-4056-81A4-75DF083A99E0}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>81</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{C294985B-E6EB-40A5-8DFE-853172BBCCB1}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F11C9F18-0D54-4C96-BED8-DE87C1369977}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1033,22 +1522,22 @@
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="B1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -1059,7 +1548,154 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5FD66FB-087A-4BE0-AD53-96903EBC09C4}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDCD33EE-0A44-410C-8DC5-C065FBFA5F79}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="43" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{4A93CEC8-FAC0-4D43-94E1-539353D8B566}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95CDEE87-BA4B-4159-A872-0FB688D1BFE4}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>79</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{67828866-220C-48B5-9D02-8AE8FB19356A}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4800AC7E-F153-4191-9E90-3380C12B1430}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{98773125-5332-4379-98B8-0FD3F271177C}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62D6A461-64F3-42C2-B275-475DA0075823}">
   <dimension ref="A1:CW2"/>
   <sheetViews>
@@ -1067,47 +1703,47 @@
       <selection activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:101">
       <c r="A1" s="4" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="N1" s="5"/>
       <c r="O1" s="5"/>
@@ -1198,45 +1834,45 @@
       <c r="CV1" s="5"/>
       <c r="CW1" s="5"/>
     </row>
-    <row r="2" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:101">
       <c r="A2" s="6" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="5" t="s">
-        <v>25</v>
-      </c>
       <c r="F2" s="5" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>28</v>
       </c>
       <c r="H2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="J2" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="K2" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="M2" s="5" t="s">
         <v>31</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="M2" s="5" t="s">
-        <v>32</v>
       </c>
       <c r="N2" s="5"/>
       <c r="O2" s="5"/>
@@ -1335,161 +1971,169 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="41.7109375" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{938664A6-98D0-4D67-82A6-5216F9BEBF97}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{984425FB-E0ED-4499-9F06-D56178AE2B8E}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="30.85546875" customWidth="1"/>
+    <col min="2" max="2" width="30" customWidth="1"/>
+    <col min="3" max="3" width="22.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{CFA4C855-DE38-4355-86BF-026061729869}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4800AC7E-F153-4191-9E90-3380C12B1430}">
-  <dimension ref="A1:A2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57C9431D-5367-4EBD-BB7D-638E4D59A5BF}">
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2">
+      <c r="A1" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>16</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{98773125-5332-4379-98B8-0FD3F271177C}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{95739FB7-D7F2-409C-8597-E9D2267B148E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DBB4210-9285-4E78-B062-C70F95124B52}">
-  <dimension ref="A1:G10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F176698D-2844-4849-825F-67D3B337053C}">
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="29.42578125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="E1" s="10" t="s">
+    <row r="1" spans="1:4">
+      <c r="A1" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="F1" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" s="10" t="s">
+      <c r="B1" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="C1" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="F2" s="10" t="s">
+      <c r="C2" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="G2" s="10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="10"/>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="10"/>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="10"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" s="10"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7" s="10"/>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" s="10"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" s="10"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A10" s="10"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{172E0C13-61F9-4032-BF55-C665681D7995}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1500,27 +2144,27 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="44.453125" customWidth="1"/>
-    <col min="2" max="2" width="15.54296875" customWidth="1"/>
-    <col min="5" max="5" width="20.1796875" customWidth="1"/>
+    <col min="1" max="1" width="44.42578125" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" customWidth="1"/>
+    <col min="5" max="5" width="20.140625" customWidth="1"/>
     <col min="8" max="8" width="14" customWidth="1"/>
-    <col min="9" max="9" width="18.26953125" customWidth="1"/>
+    <col min="9" max="9" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9">
       <c r="A1" s="9" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="C1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E1" t="s">
         <v>41</v>
@@ -1535,36 +2179,36 @@
         <v>44</v>
       </c>
       <c r="I1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>4</v>
+        <v>34</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D2" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="E2" t="s">
         <v>45</v>
       </c>
       <c r="F2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="H2" t="s">
         <v>46</v>
       </c>
       <c r="I2" t="s">
-        <v>5</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added DefectXML and TestData
</commit_message>
<xml_diff>
--- a/testData/defectTabTestData/defectTestCaseTab_testData.xlsx
+++ b/testData/defectTabTestData/defectTestCaseTab_testData.xlsx
@@ -1,16 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29530"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MohitAman\Desktop\UAT_NEXTNEXT_BLAZE_FRAMEWORK_AUTO\testData\defectTabTestData\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0816BAE2-6BDC-4123-AFF9-7CD93ADFA1E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8D63A7C1-48AE-41E4-895F-92B3370458E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="18" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="14" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tc004" sheetId="4" r:id="rId1"/>
@@ -24,29 +19,40 @@
     <sheet name="tc016" sheetId="9" r:id="rId9"/>
     <sheet name="tc017" sheetId="10" r:id="rId10"/>
     <sheet name="tc018" sheetId="17" r:id="rId11"/>
-    <sheet name="tc029" sheetId="13" r:id="rId12"/>
-    <sheet name="tc047" sheetId="18" r:id="rId13"/>
-    <sheet name="tc046" sheetId="19" r:id="rId14"/>
-    <sheet name="tc030" sheetId="14" r:id="rId15"/>
-    <sheet name="tc041" sheetId="16" r:id="rId16"/>
-    <sheet name="tc037" sheetId="21" r:id="rId17"/>
-    <sheet name="tc021" sheetId="11" r:id="rId18"/>
-    <sheet name="tc023" sheetId="12" r:id="rId19"/>
-    <sheet name="tc026" sheetId="15" r:id="rId20"/>
-    <sheet name="tc042" sheetId="22" r:id="rId21"/>
-    <sheet name="tc027" sheetId="20" r:id="rId22"/>
+    <sheet name="tc021" sheetId="11" r:id="rId12"/>
+    <sheet name="tc023" sheetId="12" r:id="rId13"/>
+    <sheet name="tc026" sheetId="15" r:id="rId14"/>
+    <sheet name="tc027" sheetId="20" r:id="rId15"/>
+    <sheet name="tc029" sheetId="13" r:id="rId16"/>
+    <sheet name="tc030" sheetId="14" r:id="rId17"/>
+    <sheet name="tc041" sheetId="16" r:id="rId18"/>
+    <sheet name="tc047" sheetId="18" r:id="rId19"/>
+    <sheet name="tc037" sheetId="24" r:id="rId20"/>
+    <sheet name="tc046" sheetId="19" r:id="rId21"/>
+    <sheet name="tc042" sheetId="23" r:id="rId22"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="85">
   <si>
     <t>project</t>
   </si>
@@ -187,27 +193,6 @@
   </si>
   <si>
     <t>Mohit Aman</t>
-  </si>
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>ID1</t>
-  </si>
-  <si>
-    <t>DF-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   Testing Summary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">status </t>
-  </si>
-  <si>
-    <t>testcase Summary</t>
-  </si>
-  <si>
-    <t>Automation Description</t>
   </si>
   <si>
     <t>defectId</t>
@@ -315,12 +300,39 @@
 Test data (if any) :
 Test case number : </t>
   </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>ID1</t>
+  </si>
+  <si>
+    <t>DF-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Testing Summary</t>
+  </si>
+  <si>
+    <t>####</t>
+  </si>
+  <si>
+    <t>&amp;&amp;&amp;&amp;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">status </t>
+  </si>
+  <si>
+    <t>testcase Summary</t>
+  </si>
+  <si>
+    <t>Automation Description</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -338,7 +350,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -368,7 +380,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -397,7 +409,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -405,6 +417,13 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -458,7 +477,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -800,7 +819,7 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="10" t="s">
@@ -933,9 +952,9 @@
       <selection sqref="A1:I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="9" max="9" width="29.1796875" customWidth="1"/>
+    <col min="9" max="9" width="29.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -1012,11 +1031,11 @@
       <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="7" max="7" width="14.453125" customWidth="1"/>
-    <col min="8" max="8" width="17.1796875" customWidth="1"/>
-    <col min="9" max="9" width="27.1796875" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" customWidth="1"/>
+    <col min="8" max="8" width="17.140625" customWidth="1"/>
+    <col min="9" max="9" width="27.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -1086,6 +1105,229 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41609440-00B7-4122-9080-D2BC0A433D51}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5:D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="60.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="115.5">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="D5" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3259BD86-3F8F-4A42-86F4-5DD744C41E44}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56806B28-3978-47F9-8A2E-A1FAB993CEA2}">
+  <dimension ref="A1:N2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="25.42578125" defaultRowHeight="55.5" customHeight="1"/>
+  <cols>
+    <col min="1" max="16384" width="25.42578125" style="16"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="55.5" customHeight="1">
+      <c r="A1" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="H1" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="I1" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="J1" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="K1" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="L1" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="M1" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1" s="15" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="55.5" customHeight="1">
+      <c r="A2" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="15"/>
+      <c r="C2" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="I2" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="J2" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="K2" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="L2" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="M2" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="N2" s="15" t="s">
+        <v>74</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8D2FA3B-A385-40DB-B8F7-3AD897BAF126}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="216.75">
+      <c r="A2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>75</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAA3B7BB-8D47-428A-AFA2-8FBE09983B20}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -1093,9 +1335,9 @@
       <selection sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4" ht="15">
+    <row r="1" spans="1:4">
       <c r="A1" s="7" t="s">
         <v>36</v>
       </c>
@@ -1109,7 +1351,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15">
+    <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
         <v>16</v>
       </c>
@@ -1131,7 +1373,102 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{291E5E8B-3DC4-459B-886A-59328C11C1BB}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{6784271E-276C-4D31-8375-14BA890EE7FF}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC29B807-E3D5-449A-8A03-0861456EF643}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView topLeftCell="K1" workbookViewId="0">
+      <selection sqref="A1:C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="50.85546875" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" customWidth="1"/>
+    <col min="3" max="3" width="27.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{C4C735ED-C70C-4B58-8CAD-3C000986EACA}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4399D2F9-CD9F-4056-81A4-75DF083A99E0}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -1139,9 +1476,9 @@
       <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4" ht="15">
+    <row r="1" spans="1:4">
       <c r="A1" s="7" t="s">
         <v>36</v>
       </c>
@@ -1155,288 +1492,24 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15">
+    <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>38</v>
+        <v>80</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>13</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>40</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{C294985B-E6EB-40A5-8DFE-853172BBCCB1}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDCD33EE-0A44-410C-8DC5-C065FBFA5F79}">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="43" defaultRowHeight="14.5"/>
-  <sheetData>
-    <row r="1" spans="1:4" ht="15">
-      <c r="A1" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="15">
-      <c r="A2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{4A93CEC8-FAC0-4D43-94E1-539353D8B566}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{291E5E8B-3DC4-459B-886A-59328C11C1BB}">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <sheetData>
-    <row r="1" spans="1:4" ht="15">
-      <c r="A1" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="15">
-      <c r="A2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{6784271E-276C-4D31-8375-14BA890EE7FF}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC29B807-E3D5-449A-8A03-0861456EF643}">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <cols>
-    <col min="1" max="1" width="50.81640625" customWidth="1"/>
-    <col min="2" max="2" width="14.26953125" customWidth="1"/>
-    <col min="3" max="3" width="27.81640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="D1" s="13" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="D2" s="14" t="s">
-        <v>49</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{C4C735ED-C70C-4B58-8CAD-3C000986EACA}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49B5ED9E-0B13-4297-A032-40A1BE654259}">
-  <dimension ref="A1:C20"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <cols>
-    <col min="1" max="1" width="20.453125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" t="s">
-        <v>1</v>
-      </c>
-      <c r="B19" t="s">
-        <v>51</v>
-      </c>
-      <c r="C19" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" t="s">
-        <v>52</v>
-      </c>
-      <c r="B20" t="s">
-        <v>13</v>
-      </c>
-      <c r="C20" t="s">
-        <v>53</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41609440-00B7-4122-9080-D2BC0A433D51}">
-  <dimension ref="A1:D5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5:D12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <cols>
-    <col min="2" max="2" width="60.453125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="116">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="D5" s="3"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3259BD86-3F8F-4A42-86F4-5DD744C41E44}">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>33</v>
-      </c>
-    </row>
-  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1449,7 +1522,7 @@
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -1476,125 +1549,104 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56806B28-3978-47F9-8A2E-A1FAB993CEA2}">
-  <dimension ref="A1:N2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5FD66FB-087A-4BE0-AD53-96903EBC09C4}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDCD33EE-0A44-410C-8DC5-C065FBFA5F79}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="43" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{4A93CEC8-FAC0-4D43-94E1-539353D8B566}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95CDEE87-BA4B-4159-A872-0FB688D1BFE4}">
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="25.453125" defaultRowHeight="55.5" customHeight="1"/>
-  <cols>
-    <col min="1" max="16384" width="25.453125" style="16"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14" ht="55.5" customHeight="1">
-      <c r="A1" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="C1" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="D1" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="E1" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="F1" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="G1" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="H1" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="I1" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="J1" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="K1" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="L1" s="15" t="s">
-        <v>68</v>
-      </c>
-      <c r="M1" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="N1" s="15" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" ht="55.5" customHeight="1">
-      <c r="A2" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="D2" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="E2" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="F2" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="G2" s="17" t="s">
-        <v>75</v>
-      </c>
-      <c r="H2" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="I2" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="J2" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="K2" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="L2" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="M2" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="N2" s="15" t="s">
-        <v>81</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{445C4733-96F3-467D-92D0-278A912B0AEA}">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="C1" s="13" t="s">
+      <c r="B1" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" s="10" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1603,57 +1655,16 @@
         <v>16</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="C2" s="13" t="s">
-        <v>50</v>
+        <v>78</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{7FA2F25E-C0D2-4F33-B9A7-4FC6A824CB83}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{67828866-220C-48B5-9D02-8AE8FB19356A}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8D2FA3B-A385-40DB-B8F7-3AD897BAF126}">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="217.5">
-      <c r="A2" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="18" t="s">
-        <v>82</v>
-      </c>
-    </row>
-  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1664,7 +1675,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
@@ -1692,7 +1703,7 @@
       <selection activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:101">
       <c r="A1" s="4" t="s">
@@ -1968,10 +1979,10 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="41.7265625" customWidth="1"/>
-    <col min="2" max="2" width="21.1796875" customWidth="1"/>
+    <col min="1" max="1" width="41.7109375" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -2012,11 +2023,11 @@
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="30.81640625" customWidth="1"/>
+    <col min="1" max="1" width="30.85546875" customWidth="1"/>
     <col min="2" max="2" width="30" customWidth="1"/>
-    <col min="3" max="3" width="22.453125" customWidth="1"/>
+    <col min="3" max="3" width="22.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -2055,9 +2066,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" ht="15">
+    <row r="1" spans="1:2">
       <c r="A1" s="7" t="s">
         <v>36</v>
       </c>
@@ -2065,7 +2076,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15">
+    <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
         <v>16</v>
       </c>
@@ -2089,9 +2100,9 @@
       <selection sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="29.453125" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="29.42578125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4" ht="15">
+    <row r="1" spans="1:4">
       <c r="A1" s="7" t="s">
         <v>36</v>
       </c>
@@ -2105,7 +2116,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15">
+    <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
         <v>16</v>
       </c>
@@ -2133,13 +2144,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="44.453125" customWidth="1"/>
-    <col min="2" max="2" width="15.54296875" customWidth="1"/>
-    <col min="5" max="5" width="20.1796875" customWidth="1"/>
+    <col min="1" max="1" width="44.42578125" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" customWidth="1"/>
+    <col min="5" max="5" width="20.140625" customWidth="1"/>
     <col min="8" max="8" width="14" customWidth="1"/>
-    <col min="9" max="9" width="18.26953125" customWidth="1"/>
+    <col min="9" max="9" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">

</xml_diff>

<commit_message>
Dont merge this commit
</commit_message>
<xml_diff>
--- a/testData/defectTabTestData/defectTestCaseTab_testData.xlsx
+++ b/testData/defectTabTestData/defectTestCaseTab_testData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29530"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8D63A7C1-48AE-41E4-895F-92B3370458E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5976FE54-119D-46F3-935F-DD1876017DD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="14" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="16" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tc004" sheetId="4" r:id="rId1"/>
@@ -23,13 +23,15 @@
     <sheet name="tc023" sheetId="12" r:id="rId13"/>
     <sheet name="tc026" sheetId="15" r:id="rId14"/>
     <sheet name="tc027" sheetId="20" r:id="rId15"/>
-    <sheet name="tc029" sheetId="13" r:id="rId16"/>
-    <sheet name="tc030" sheetId="14" r:id="rId17"/>
-    <sheet name="tc041" sheetId="16" r:id="rId18"/>
-    <sheet name="tc047" sheetId="18" r:id="rId19"/>
-    <sheet name="tc037" sheetId="24" r:id="rId20"/>
-    <sheet name="tc046" sheetId="19" r:id="rId21"/>
-    <sheet name="tc042" sheetId="23" r:id="rId22"/>
+    <sheet name="tc011" sheetId="25" r:id="rId16"/>
+    <sheet name="tc013" sheetId="26" r:id="rId17"/>
+    <sheet name="tc029" sheetId="13" r:id="rId18"/>
+    <sheet name="tc030" sheetId="14" r:id="rId19"/>
+    <sheet name="tc041" sheetId="16" r:id="rId20"/>
+    <sheet name="tc047" sheetId="18" r:id="rId21"/>
+    <sheet name="tc037" sheetId="24" r:id="rId22"/>
+    <sheet name="tc046" sheetId="19" r:id="rId23"/>
+    <sheet name="tc042" sheetId="23" r:id="rId24"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -52,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="90">
   <si>
     <t>project</t>
   </si>
@@ -301,10 +303,25 @@
 Test case number : </t>
   </si>
   <si>
+    <t>Summary123!@#</t>
+  </si>
+  <si>
+    <t>affectedRelease</t>
+  </si>
+  <si>
+    <t>module</t>
+  </si>
+  <si>
+    <t>severity</t>
+  </si>
+  <si>
+    <t>Release 039</t>
+  </si>
+  <si>
+    <t>Cosmetic</t>
+  </si>
+  <si>
     <t>ID</t>
-  </si>
-  <si>
-    <t>ID1</t>
   </si>
   <si>
     <t>DF-1</t>
@@ -332,7 +349,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -401,18 +418,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -424,6 +429,12 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FFBCBEC4"/>
+      <name val="Courier New"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="2">
@@ -447,7 +458,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -463,21 +474,20 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1192,92 +1202,92 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.42578125" defaultRowHeight="55.5" customHeight="1"/>
   <cols>
-    <col min="1" max="16384" width="25.42578125" style="16"/>
+    <col min="1" max="16384" width="25.42578125" style="14"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="55.5" customHeight="1">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F1" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="G1" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="H1" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="I1" s="15" t="s">
+      <c r="I1" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="J1" s="15" t="s">
+      <c r="J1" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="K1" s="15" t="s">
+      <c r="K1" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="L1" s="15" t="s">
+      <c r="L1" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="M1" s="15" t="s">
+      <c r="M1" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="N1" s="15" t="s">
+      <c r="N1" s="13" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="55.5" customHeight="1">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="17" t="s">
+      <c r="B2" s="13"/>
+      <c r="C2" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="E2" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="F2" s="17" t="s">
+      <c r="F2" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="G2" s="17" t="s">
+      <c r="G2" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="H2" s="17" t="s">
+      <c r="H2" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="I2" s="17" t="s">
+      <c r="I2" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="J2" s="17" t="s">
+      <c r="J2" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="K2" s="17" t="s">
+      <c r="K2" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="L2" s="17" t="s">
+      <c r="L2" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="M2" s="17" t="s">
+      <c r="M2" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="N2" s="15" t="s">
+      <c r="N2" s="13" t="s">
         <v>74</v>
       </c>
     </row>
@@ -1290,7 +1300,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8D2FA3B-A385-40DB-B8F7-3AD897BAF126}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
@@ -1312,13 +1322,13 @@
       <c r="A2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="16" t="s">
         <v>32</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="16" t="s">
         <v>75</v>
       </c>
     </row>
@@ -1328,6 +1338,76 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47BC1E89-27CE-4864-90F3-20162B3719B5}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="8"/>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{484D8939-7FDB-49ED-81B6-808A8C8953E5}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>81</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAA3B7BB-8D47-428A-AFA2-8FBE09983B20}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -1373,7 +1453,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{291E5E8B-3DC4-459B-886A-59328C11C1BB}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -1417,12 +1497,46 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F11C9F18-0D54-4C96-BED8-DE87C1369977}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{2526BF51-A6FB-47A9-8E2C-36ED1636F3F4}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC29B807-E3D5-449A-8A03-0861456EF643}">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView topLeftCell="K1" workbookViewId="0">
-      <selection sqref="A1:C2"/>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1432,51 +1546,128 @@
     <col min="3" max="3" width="27.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:3">
       <c r="A1" s="9" t="s">
         <v>14</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="C1" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="D1" s="13" t="s">
-        <v>77</v>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>84</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{C4C735ED-C70C-4B58-8CAD-3C000986EACA}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4399D2F9-CD9F-4056-81A4-75DF083A99E0}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="D2" s="14" t="s">
-        <v>78</v>
+      <c r="B2" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{C4C735ED-C70C-4B58-8CAD-3C000986EACA}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{C294985B-E6EB-40A5-8DFE-853172BBCCB1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4399D2F9-CD9F-4056-81A4-75DF083A99E0}">
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5FD66FB-087A-4BE0-AD53-96903EBC09C4}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>89</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDCD33EE-0A44-410C-8DC5-C065FBFA5F79}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="43" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="7" t="s">
@@ -1497,123 +1688,6 @@
         <v>16</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>81</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{C294985B-E6EB-40A5-8DFE-853172BBCCB1}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F11C9F18-0D54-4C96-BED8-DE87C1369977}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{2526BF51-A6FB-47A9-8E2C-36ED1636F3F4}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5FD66FB-087A-4BE0-AD53-96903EBC09C4}">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>84</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDCD33EE-0A44-410C-8DC5-C065FBFA5F79}">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="43" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" s="8" t="s">
         <v>38</v>
       </c>
       <c r="C2" s="8" t="s">
@@ -1631,7 +1705,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95CDEE87-BA4B-4159-A872-0FB688D1BFE4}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -1644,7 +1718,7 @@
         <v>14</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="C1" s="10" t="s">
         <v>32</v>
@@ -1654,11 +1728,11 @@
       <c r="A2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="19" t="s">
-        <v>78</v>
+      <c r="B2" s="17" t="s">
+        <v>83</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added New method for SelctDropdown using index
</commit_message>
<xml_diff>
--- a/testData/defectTabTestData/defectTestCaseTab_testData.xlsx
+++ b/testData/defectTabTestData/defectTestCaseTab_testData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29602"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{385BECE3-6654-413B-B90C-8708DBBC451F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A4323110-878E-4DDF-8D03-0B7029A4ED8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="10" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="94">
   <si>
     <t>project</t>
   </si>
@@ -197,12 +197,6 @@
   </si>
   <si>
     <t>Assign To</t>
-  </si>
-  <si>
-    <t>Requirement - Wrong</t>
-  </si>
-  <si>
-    <t>Mohit Aman</t>
   </si>
   <si>
     <t>defectId</t>
@@ -1001,7 +995,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1042,20 +1036,20 @@
       <c r="B2" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E2" t="s">
-        <v>35</v>
-      </c>
-      <c r="F2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" t="s">
-        <v>48</v>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>12</v>
       </c>
       <c r="H2" t="s">
         <v>21</v>
@@ -1074,7 +1068,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1117,20 +1111,20 @@
       <c r="B2" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E2" t="s">
-        <v>35</v>
-      </c>
-      <c r="F2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" t="s">
-        <v>48</v>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>12</v>
       </c>
       <c r="H2" t="s">
         <v>21</v>
@@ -1159,10 +1153,10 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="115.5">
@@ -1170,7 +1164,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1240,43 +1234,43 @@
         <v>0</v>
       </c>
       <c r="B1" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="E1" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="F1" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="G1" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="H1" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="I1" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="J1" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="K1" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="L1" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="K1" s="10" t="s">
+      <c r="M1" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="L1" s="10" t="s">
+      <c r="N1" s="10" t="s">
         <v>62</v>
-      </c>
-      <c r="M1" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="N1" s="10" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="55.5" customHeight="1">
@@ -1285,40 +1279,40 @@
       </c>
       <c r="B2" s="10"/>
       <c r="C2" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="E2" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="F2" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="G2" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="H2" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="I2" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="J2" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="K2" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="I2" s="12" t="s">
+      <c r="L2" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="J2" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="K2" s="12" t="s">
+      <c r="M2" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="L2" s="12" t="s">
+      <c r="N2" s="10" t="s">
         <v>73</v>
-      </c>
-      <c r="M2" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="N2" s="10" t="s">
-        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -1359,7 +1353,7 @@
         <v>13</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -1391,7 +1385,7 @@
         <v>13</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C2" s="5"/>
     </row>
@@ -1412,24 +1406,24 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>78</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1458,21 +1452,21 @@
         <v>38</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -1492,24 +1486,24 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>13</v>
@@ -1521,7 +1515,7 @@
         <v>35</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -1673,7 +1667,7 @@
         <v>14</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>18</v>
@@ -1684,10 +1678,10 @@
         <v>16</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -1727,13 +1721,13 @@
         <v>16</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -1759,7 +1753,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>19</v>
@@ -1767,13 +1761,13 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -1840,7 +1834,7 @@
         <v>14</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>18</v>
@@ -1851,10 +1845,10 @@
         <v>16</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -2177,7 +2171,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2222,20 +2216,20 @@
       <c r="B2" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E2" t="s">
-        <v>35</v>
-      </c>
-      <c r="F2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" t="s">
-        <v>48</v>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>12</v>
       </c>
       <c r="H2" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
Changed in the dataprovider
</commit_message>
<xml_diff>
--- a/testData/defectTabTestData/defectTestCaseTab_testData.xlsx
+++ b/testData/defectTabTestData/defectTestCaseTab_testData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MohitAman\Desktop\UAT_NEXTNEXT_BLAZE_FRAMEWORK_AUTO\testData\defectTabTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5C6F065-7324-4DAF-9F8B-5B5E1B46CBBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF50CDF7-7ADA-44E9-9075-CB71FA436ABE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="8" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="94">
   <si>
     <t>project</t>
   </si>
@@ -979,19 +979,19 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87E5D401-1490-449E-9C0A-3DF35853EE92}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:H2"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="27.81640625" customWidth="1"/>
-    <col min="8" max="8" width="29.1796875" customWidth="1"/>
+    <col min="3" max="3" width="29.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:3">
       <c r="A1" s="6" t="s">
         <v>14</v>
       </c>
@@ -999,47 +999,17 @@
         <v>18</v>
       </c>
       <c r="C1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F1" t="s">
-        <v>45</v>
-      </c>
-      <c r="G1" t="s">
-        <v>46</v>
-      </c>
-      <c r="H1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>2</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2">
-        <v>12</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="C2" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated test cases TC011 TC033
</commit_message>
<xml_diff>
--- a/testData/defectTabTestData/defectTestCaseTab_testData.xlsx
+++ b/testData/defectTabTestData/defectTestCaseTab_testData.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29602"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:dbsheet="http://web.wps.cn/et/2021/dbsheet">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A4323110-878E-4DDF-8D03-0B7029A4ED8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="10" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="18600" windowHeight="6080" firstSheet="16" activeTab="25"/>
   </bookViews>
   <sheets>
     <sheet name="tc004" sheetId="4" r:id="rId1"/>
@@ -23,23 +22,20 @@
     <sheet name="tc023" sheetId="12" r:id="rId13"/>
     <sheet name="tc026" sheetId="15" r:id="rId14"/>
     <sheet name="tc027" sheetId="20" r:id="rId15"/>
-    <sheet name="tc011" sheetId="25" r:id="rId16"/>
-    <sheet name="tc013" sheetId="26" r:id="rId17"/>
-    <sheet name="tc033" sheetId="27" r:id="rId18"/>
-    <sheet name="tc035" sheetId="28" r:id="rId19"/>
-    <sheet name="tc029" sheetId="13" r:id="rId20"/>
-    <sheet name="tc030" sheetId="14" r:id="rId21"/>
-    <sheet name="tc041" sheetId="16" r:id="rId22"/>
-    <sheet name="tc047" sheetId="18" r:id="rId23"/>
-    <sheet name="tc037" sheetId="24" r:id="rId24"/>
-    <sheet name="tc046" sheetId="19" r:id="rId25"/>
-    <sheet name="tc042" sheetId="23" r:id="rId26"/>
+    <sheet name="tc013" sheetId="26" r:id="rId16"/>
+    <sheet name="tc033" sheetId="27" r:id="rId17"/>
+    <sheet name="tc035" sheetId="28" r:id="rId18"/>
+    <sheet name="tc029" sheetId="13" r:id="rId19"/>
+    <sheet name="tc030" sheetId="14" r:id="rId20"/>
+    <sheet name="tc041" sheetId="16" r:id="rId21"/>
+    <sheet name="tc047" sheetId="18" r:id="rId22"/>
+    <sheet name="tc037" sheetId="24" r:id="rId23"/>
+    <sheet name="tc046" sheetId="19" r:id="rId24"/>
+    <sheet name="tc042" sheetId="23" r:id="rId25"/>
+    <sheet name="tc011" sheetId="30" r:id="rId26"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -56,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="94">
   <si>
     <t>project</t>
   </si>
@@ -302,121 +298,113 @@
 Test case number : </t>
   </si>
   <si>
+    <t>affectedRelease</t>
+  </si>
+  <si>
+    <t>module</t>
+  </si>
+  <si>
+    <t>severity</t>
+  </si>
+  <si>
+    <t>Release 039</t>
+  </si>
+  <si>
+    <t>Cosmetic</t>
+  </si>
+  <si>
+    <t>summary2</t>
+  </si>
+  <si>
+    <t>User is unable to save the status.</t>
+  </si>
+  <si>
+    <t>XX</t>
+  </si>
+  <si>
+    <t>assigned_To</t>
+  </si>
+  <si>
+    <t>Arkajit Tah</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>DF-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Testing Summary</t>
+  </si>
+  <si>
+    <t>####</t>
+  </si>
+  <si>
+    <t>&amp;&amp;&amp;&amp;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">status </t>
+  </si>
+  <si>
+    <t>testcase Summary</t>
+  </si>
+  <si>
+    <t>Automation Description</t>
+  </si>
+  <si>
     <t>Summary123!@#</t>
-  </si>
-  <si>
-    <t>affectedRelease</t>
-  </si>
-  <si>
-    <t>module</t>
-  </si>
-  <si>
-    <t>severity</t>
-  </si>
-  <si>
-    <t>Release 039</t>
-  </si>
-  <si>
-    <t>Cosmetic</t>
-  </si>
-  <si>
-    <t>summary2</t>
-  </si>
-  <si>
-    <t>User is unable to save the status.</t>
-  </si>
-  <si>
-    <t>XX</t>
-  </si>
-  <si>
-    <t>assigned_To</t>
-  </si>
-  <si>
-    <t>Arkajit Tah</t>
-  </si>
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>DF-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   Testing Summary</t>
-  </si>
-  <si>
-    <t>####</t>
-  </si>
-  <si>
-    <t>&amp;&amp;&amp;&amp;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">status </t>
-  </si>
-  <si>
-    <t>testcase Summary</t>
-  </si>
-  <si>
-    <t>Automation Description</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
+  <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="30">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color theme="10"/>
       <name val="Aptos Narrow"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Aptos Narrow"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF242424"/>
-      <name val="Calibri"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -427,15 +415,8 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9.8000000000000007"/>
-      <color rgb="FFBCBEC4"/>
-      <name val="Courier New"/>
+      <color rgb="FF242424"/>
+      <name val="Calibri"/>
       <charset val="134"/>
     </font>
     <font>
@@ -450,8 +431,157 @@
       <name val="Calibri"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Aptos Narrow"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Aptos Narrow"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Aptos Narrow"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Aptos Narrow"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Aptos Narrow"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -464,8 +594,194 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -488,55 +804,335 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="176" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="6"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="6" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="6" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="6" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" quotePrefix="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
+    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
+    <cellStyle name="Link" xfId="6" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
+    <cellStyle name="Note" xfId="8" builtinId="10"/>
+    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
+    <cellStyle name="Title" xfId="10" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
+    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
+    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
+    <cellStyle name="Input" xfId="16" builtinId="20"/>
+    <cellStyle name="Output" xfId="17" builtinId="21"/>
+    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
+    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
+    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
+    <cellStyle name="Total" xfId="21" builtinId="25"/>
+    <cellStyle name="Good" xfId="22" builtinId="26"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
+    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -585,7 +1181,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Aptos Display" panose="020F0302020204030204"/>
+        <a:latin typeface="Aptos Display"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -618,26 +1214,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
+        <a:latin typeface="Aptos Narrow"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -670,23 +1249,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -848,166 +1410,163 @@
       </a:style>
     </a:lnDef>
   </a:objectDefaults>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DBB4210-9285-4E78-B062-C70F95124B52}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="6"/>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" s="7" t="s">
+    <row r="1" ht="14.5" spans="1:7">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="7" t="s">
+    <row r="2" ht="14.5" spans="1:7">
+      <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="7"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="7"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="7"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="7"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
+    <row r="3" ht="14.5" spans="1:7">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" ht="14.5" spans="1:7">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" ht="14.5" spans="1:7">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" ht="14.5" spans="1:7">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" ht="14.5" spans="1:7">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" ht="14.5" spans="1:7">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" ht="14.5" spans="1:7">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+    </row>
+    <row r="10" ht="14.5" spans="1:7">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87E5D401-1490-449E-9C0A-3DF35853EE92}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="7"/>
   <cols>
-    <col min="8" max="8" width="29.140625" customWidth="1"/>
+    <col min="8" max="8" width="29.1363636363636" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C1" t="s">
@@ -1030,10 +1589,10 @@
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>20</v>
       </c>
       <c r="C2">
@@ -1057,32 +1616,34 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{B9D4C0EB-7FDD-4EC8-8600-7F09218EAE8D}"/>
+    <hyperlink ref="A2" r:id="rId1" display="https://webapp-stg-testnext.azurewebsites.net/defect"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B310B858-FEFA-48A5-B995-DA133501E07F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="7"/>
   <cols>
-    <col min="6" max="6" width="14.42578125" customWidth="1"/>
-    <col min="7" max="7" width="17.140625" customWidth="1"/>
-    <col min="8" max="8" width="27.140625" customWidth="1"/>
+    <col min="6" max="6" width="14.4272727272727" customWidth="1"/>
+    <col min="7" max="7" width="17.1363636363636" customWidth="1"/>
+    <col min="8" max="8" width="27.1363636363636" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C1" t="s">
@@ -1105,10 +1666,10 @@
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>20</v>
       </c>
       <c r="C2">
@@ -1132,26 +1693,28 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{AB19A363-286C-4679-8DCD-0C56253EB022}"/>
+    <hyperlink ref="A2" r:id="rId1" display="https://webapp-stg-testnext.azurewebsites.net/defect"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41609440-00B7-4122-9080-D2BC0A433D51}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5:D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="4" outlineLevelCol="3"/>
   <cols>
-    <col min="2" max="2" width="60.42578125" customWidth="1"/>
+    <col min="2" max="2" width="60.4272727272727" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>47</v>
       </c>
@@ -1159,379 +1722,412 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="115.5">
+    <row r="2" ht="112" spans="1:2">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="11" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
-      <c r="D5" s="3"/>
+    <row r="5" spans="4:4">
+      <c r="D5" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3259BD86-3F8F-4A42-86F4-5DD744C41E44}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="3"/>
+  <sheetData>
+    <row r="1" ht="14.5" spans="1:4">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" ht="14.5" spans="1:4">
+      <c r="A2" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:N2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="25.4272727272727" defaultRowHeight="55.5" customHeight="1" outlineLevelRow="1"/>
+  <cols>
+    <col min="1" max="16384" width="25.4272727272727" style="8"/>
+  </cols>
+  <sheetData>
+    <row r="1" customHeight="1" spans="1:14">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="K1" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="L1" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="M1" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="N1" s="9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" customHeight="1" spans="1:14">
+      <c r="A2" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="9"/>
+      <c r="C2" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="I2" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="J2" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="K2" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="L2" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="M2" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="N2" s="9" t="s">
+        <v>73</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="3"/>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="8" t="s">
+    <row r="2" ht="238" spans="1:4">
+      <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>19</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56806B28-3978-47F9-8A2E-A1FAB993CEA2}">
-  <dimension ref="A1:N2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="25.42578125" defaultRowHeight="55.5" customHeight="1"/>
-  <cols>
-    <col min="1" max="16384" width="25.42578125" style="11"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14" ht="55.5" customHeight="1">
-      <c r="A1" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="I1" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="J1" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="K1" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="L1" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="M1" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="N1" s="10" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" ht="55.5" customHeight="1">
-      <c r="A2" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="F2" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="G2" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="H2" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="I2" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="J2" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="K2" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="L2" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="M2" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="N2" s="10" t="s">
-        <v>73</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8D2FA3B-A385-40DB-B8F7-3AD897BAF126}">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="216.75">
-      <c r="A2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>74</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47BC1E89-27CE-4864-90F3-20162B3719B5}">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="5"/>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="C2" s="5"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{484D8939-7FDB-49ED-81B6-808A8C8953E5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="2"/>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C1" s="5" t="s">
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="5" t="s">
+      <c r="B2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>80</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{151DEB7C-D179-49F8-97B3-BE1831536417}">
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="3"/>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="5" t="s">
+      <c r="B2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>82</v>
+      <c r="D2" s="1" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CC0CE84-E866-472B-BB42-2AAD8AE92A1A}">
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="4"/>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="B1" s="5" t="s">
+      <c r="A1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D1" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="5" t="s">
+      <c r="B2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>84</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>85</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="$A1:$XFD2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="3"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="https://webapp-stg-testnext.azurewebsites.net/defect"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F11C9F18-0D54-4C96-BED8-DE87C1369977}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="1"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -1542,7 +2138,7 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B2" t="s">
@@ -1551,321 +2147,331 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{2526BF51-A6FB-47A9-8E2C-36ED1636F3F4}"/>
+    <hyperlink ref="A2" r:id="rId1" display="https://webapp-stg-testnext.azurewebsites.net/defect"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAA3B7BB-8D47-428A-AFA2-8FBE09983B20}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD2"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="3"/>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="1" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="1" t="s">
         <v>42</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{37AC72DE-8FBE-4EDB-8A35-CE96D7521365}"/>
+    <hyperlink ref="A2" r:id="rId1" display="https://webapp-stg-testnext.azurewebsites.net/defect"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{291E5E8B-3DC4-459B-886A-59328C11C1BB}">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{6784271E-276C-4D31-8375-14BA890EE7FF}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC29B807-E3D5-449A-8A03-0861456EF643}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C2"/>
+      <selection activeCell="A1" sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="50.85546875" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" customWidth="1"/>
-    <col min="3" max="3" width="27.85546875" customWidth="1"/>
+    <col min="1" max="1" width="50.8545454545455" customWidth="1"/>
+    <col min="2" max="2" width="14.2818181818182" customWidth="1"/>
+    <col min="3" max="3" width="27.8545454545455" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" s="9" t="s">
+      <c r="C2" s="5" t="s">
         <v>87</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>88</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{C4C735ED-C70C-4B58-8CAD-3C000986EACA}"/>
+    <hyperlink ref="A2" r:id="rId1" display="https://webapp-stg-testnext.azurewebsites.net/defect"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4399D2F9-CD9F-4056-81A4-75DF083A99E0}">
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="3"/>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="1" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>90</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{C294985B-E6EB-40A5-8DFE-853172BBCCB1}"/>
+    <hyperlink ref="A2" r:id="rId1" display="https://webapp-stg-testnext.azurewebsites.net/defect"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5FD66FB-087A-4BE0-AD53-96903EBC09C4}">
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C2"/>
+      <selection activeCell="A1" sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="2"/>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="5" t="s">
+      <c r="B2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>93</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDCD33EE-0A44-410C-8DC5-C065FBFA5F79}">
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="43" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="43" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="3"/>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="1" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="1" t="s">
         <v>42</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{4A93CEC8-FAC0-4D43-94E1-539353D8B566}"/>
+    <hyperlink ref="A2" r:id="rId1" display="https://webapp-stg-testnext.azurewebsites.net/defect"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95CDEE87-BA4B-4159-A872-0FB688D1BFE4}">
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="2"/>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="7" t="s">
+    <row r="1" ht="14.5" spans="1:3">
+      <c r="A1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" ht="14.5" spans="1:3">
+      <c r="A2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="C1" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" s="14" t="s">
+      <c r="C2" s="2" t="s">
         <v>87</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>88</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{67828866-220C-48B5-9D02-8AE8FB19356A}"/>
+    <hyperlink ref="A2" r:id="rId1" display="https://webapp-stg-testnext.azurewebsites.net/defect"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="1"/>
+  <cols>
+    <col min="2" max="2" width="15.2727272727273" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4800AC7E-F153-4191-9E90-3380C12B1430}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
@@ -1873,30 +2479,32 @@
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>16</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{98773125-5332-4379-98B8-0FD3F271177C}"/>
+    <hyperlink ref="A2" r:id="rId1" display="https://webapp-stg-testnext.azurewebsites.net/defect"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="41.7109375" customWidth="1"/>
-    <col min="2" max="2" width="21.140625" customWidth="1"/>
+    <col min="1" max="1" width="41.7090909090909" customWidth="1"/>
+    <col min="2" max="2" width="21.1363636363636" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1911,7 +2519,7 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B2" t="s">
@@ -1923,25 +2531,27 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{938664A6-98D0-4D67-82A6-5216F9BEBF97}"/>
+    <hyperlink ref="A2" r:id="rId1" display="https://webapp-stg-testnext.azurewebsites.net/defect"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{984425FB-E0ED-4499-9F06-D56178AE2B8E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="30.85546875" customWidth="1"/>
+    <col min="1" max="1" width="30.8545454545455" customWidth="1"/>
     <col min="2" max="2" width="30" customWidth="1"/>
-    <col min="3" max="3" width="22.42578125" customWidth="1"/>
+    <col min="3" max="3" width="22.4272727272727" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1956,238 +2566,246 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="16" t="s">
         <v>16</v>
       </c>
       <c r="B2" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="11" t="s">
         <v>21</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{CFA4C855-DE38-4355-86BF-026061729869}"/>
+    <hyperlink ref="A2" r:id="rId1" display="https://webapp-stg-testnext.azurewebsites.net/defect"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF62085B-EB17-4E72-8097-DEB2C8E971B5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="15" defaultRowHeight="14" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="16384" width="15" style="16"/>
+    <col min="1" max="16384" width="15" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
-      <c r="A1" s="17" t="s">
+    <row r="1" ht="14.5" spans="1:13">
+      <c r="A1" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="F1" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="G1" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="18" t="s">
+      <c r="H1" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="18" t="s">
+      <c r="I1" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="J1" s="18" t="s">
+      <c r="J1" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="18" t="s">
+      <c r="K1" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="L1" s="18" t="s">
+      <c r="L1" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="18" t="s">
+      <c r="M1" s="14" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
-      <c r="A2" s="19" t="s">
+    <row r="2" ht="14.5" spans="1:13">
+      <c r="A2" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="E2" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="F2" s="18" t="s">
+      <c r="F2" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="18" t="s">
+      <c r="G2" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="H2" s="18" t="s">
+      <c r="H2" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="18" t="s">
+      <c r="I2" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="J2" s="18" t="s">
+      <c r="J2" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="K2" s="18" t="s">
+      <c r="K2" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="L2" s="18" t="s">
+      <c r="L2" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="M2" s="18" t="s">
+      <c r="M2" s="14" t="s">
         <v>35</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{C2C43611-9FF1-4030-9070-7939D6470EEA}"/>
+    <hyperlink ref="A2" r:id="rId1" display="https://webapp-stg-testnext.azurewebsites.net/defect"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57C9431D-5367-4EBD-BB7D-638E4D59A5BF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="24.42578125" customWidth="1"/>
+    <col min="1" max="1" width="24.4272727272727" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="1" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="1" t="s">
         <v>40</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{1BCD03C9-5D95-44E8-8E30-CD0AA69D5F14}"/>
+    <hyperlink ref="A2" r:id="rId1" display="https://webapp-stg-testnext.azurewebsites.net/defect"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F176698D-2844-4849-825F-67D3B337053C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C2"/>
+      <selection activeCell="A1" sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="29.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="29.4272727272727" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="3"/>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="1" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="1" t="s">
         <v>42</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{172E0C13-61F9-4032-BF55-C665681D7995}"/>
+    <hyperlink ref="A2" r:id="rId1" display="https://webapp-stg-testnext.azurewebsites.net/defect"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3D4B51D-576B-4DA1-BDAE-6F85096314D0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="1" width="44.42578125" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" customWidth="1"/>
-    <col min="4" max="4" width="20.140625" customWidth="1"/>
+    <col min="1" max="1" width="44.4272727272727" customWidth="1"/>
+    <col min="2" max="2" width="15.5727272727273" customWidth="1"/>
+    <col min="4" max="4" width="20.1363636363636" customWidth="1"/>
     <col min="7" max="7" width="14" customWidth="1"/>
-    <col min="8" max="8" width="18.28515625" customWidth="1"/>
+    <col min="8" max="8" width="18.2818181818182" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C1" t="s">
@@ -2210,10 +2828,10 @@
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>20</v>
       </c>
       <c r="C2">
@@ -2237,8 +2855,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{79DE2057-255F-4088-8F5E-0E08F75750CC}"/>
+    <hyperlink ref="A2" r:id="rId1" display="https://webapp-stg-testnext.azurewebsites.net/defect"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>